<commit_message>
Topic distribution plots in specialized media
</commit_message>
<xml_diff>
--- a/results/media_coverage.xlsx
+++ b/results/media_coverage.xlsx
@@ -400,11 +400,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E2">
         <v>84</v>
       </c>
@@ -425,11 +420,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E3">
         <v>14</v>
       </c>
@@ -450,11 +440,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E4">
         <v>80</v>
       </c>
@@ -475,11 +460,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E5">
         <v>1</v>
       </c>
@@ -500,11 +480,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E6">
         <v>1</v>
       </c>
@@ -525,11 +500,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E7">
         <v>3</v>
       </c>
@@ -550,11 +520,6 @@
           <t>Vatican</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E8">
         <v>1</v>
       </c>
@@ -575,11 +540,6 @@
           <t>Vatican</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E9">
         <v>2</v>
       </c>
@@ -600,11 +560,6 @@
           <t>Vatican</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E10">
         <v>3</v>
       </c>
@@ -650,11 +605,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E12">
         <v>1</v>
       </c>
@@ -675,11 +625,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E13">
         <v>3</v>
       </c>
@@ -700,11 +645,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E14">
         <v>1</v>
       </c>
@@ -775,11 +715,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E17">
         <v>2</v>
       </c>
@@ -800,11 +735,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E18">
         <v>2</v>
       </c>
@@ -875,11 +805,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E21">
         <v>34</v>
       </c>
@@ -900,11 +825,6 @@
           <t>Qatar</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E22">
         <v>1</v>
       </c>
@@ -1125,11 +1045,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E31">
         <v>3</v>
       </c>
@@ -1150,11 +1065,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E32">
         <v>2</v>
       </c>
@@ -1175,11 +1085,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E33">
         <v>1</v>
       </c>
@@ -1200,11 +1105,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E34">
         <v>1</v>
       </c>
@@ -1525,11 +1425,6 @@
           <t>Nicaragua</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E47">
         <v>1</v>
       </c>
@@ -1550,11 +1445,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E48">
         <v>138</v>
       </c>
@@ -1575,11 +1465,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E49">
         <v>62</v>
       </c>
@@ -1650,11 +1535,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E52">
         <v>1</v>
       </c>
@@ -1725,11 +1605,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E55">
         <v>1</v>
       </c>
@@ -1775,11 +1650,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E57">
         <v>5</v>
       </c>
@@ -1800,11 +1670,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E58">
         <v>1</v>
       </c>
@@ -1825,11 +1690,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E59">
         <v>2</v>
       </c>
@@ -1850,11 +1710,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E60">
         <v>2</v>
       </c>
@@ -1875,11 +1730,6 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E61">
         <v>4</v>
       </c>
@@ -1925,11 +1775,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E63">
         <v>1</v>
       </c>
@@ -1950,11 +1795,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E64">
         <v>356</v>
       </c>
@@ -1975,11 +1815,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E65">
         <v>1</v>
       </c>
@@ -2025,11 +1860,6 @@
           <t>Northern Ireland</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E67">
         <v>1</v>
       </c>
@@ -2050,11 +1880,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E68">
         <v>3</v>
       </c>
@@ -2075,11 +1900,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E69">
         <v>6</v>
       </c>
@@ -2100,11 +1920,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E70">
         <v>1</v>
       </c>
@@ -2150,11 +1965,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E72">
         <v>1</v>
       </c>
@@ -2200,11 +2010,6 @@
           <t>Brazil</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E74">
         <v>1</v>
       </c>
@@ -2225,11 +2030,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E75">
         <v>1</v>
       </c>
@@ -2250,11 +2050,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E76">
         <v>1</v>
       </c>
@@ -2375,11 +2170,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E81">
         <v>1</v>
       </c>
@@ -2400,11 +2190,6 @@
           <t>Canada</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E82">
         <v>1</v>
       </c>
@@ -2450,11 +2235,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E84">
         <v>130</v>
       </c>
@@ -2475,11 +2255,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E85">
         <v>2</v>
       </c>
@@ -2525,11 +2300,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E87">
         <v>2</v>
       </c>
@@ -2560,11 +2330,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E89">
         <v>33</v>
       </c>
@@ -2685,11 +2450,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E94">
         <v>1</v>
       </c>
@@ -2710,11 +2470,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E95">
         <v>4</v>
       </c>
@@ -2785,11 +2540,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E98">
         <v>2</v>
       </c>
@@ -2810,11 +2560,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E99">
         <v>1</v>
       </c>
@@ -2910,11 +2655,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E103">
         <v>2</v>
       </c>
@@ -3135,11 +2875,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E112">
         <v>13</v>
       </c>
@@ -3185,11 +2920,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E114">
         <v>2</v>
       </c>
@@ -3210,11 +2940,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E115">
         <v>2</v>
       </c>
@@ -3235,11 +2960,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E116">
         <v>1</v>
       </c>
@@ -3260,11 +2980,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E117">
         <v>5</v>
       </c>
@@ -3285,11 +3000,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E118">
         <v>1</v>
       </c>
@@ -3310,11 +3020,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E119">
         <v>1</v>
       </c>
@@ -3335,11 +3040,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E120">
         <v>2</v>
       </c>
@@ -3410,11 +3110,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E123">
         <v>3</v>
       </c>
@@ -3460,11 +3155,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E125">
         <v>2</v>
       </c>
@@ -3510,11 +3200,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E127">
         <v>1</v>
       </c>
@@ -3635,11 +3320,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E132">
         <v>3</v>
       </c>
@@ -3660,11 +3340,6 @@
           <t>Sweden</t>
         </is>
       </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E133">
         <v>1</v>
       </c>
@@ -3685,11 +3360,6 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E134">
         <v>3</v>
       </c>
@@ -3710,11 +3380,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E135">
         <v>3</v>
       </c>
@@ -3785,11 +3450,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E138">
         <v>1</v>
       </c>
@@ -3810,11 +3470,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E139">
         <v>1</v>
       </c>
@@ -3860,11 +3515,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E141">
         <v>1</v>
       </c>
@@ -3910,11 +3560,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E143">
         <v>69</v>
       </c>
@@ -3935,11 +3580,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E144">
         <v>7</v>
       </c>
@@ -3985,11 +3625,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E146">
         <v>3</v>
       </c>
@@ -4010,11 +3645,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E147">
         <v>1</v>
       </c>
@@ -4035,11 +3665,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E148">
         <v>488</v>
       </c>
@@ -4060,11 +3685,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E149">
         <v>64</v>
       </c>
@@ -4085,11 +3705,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E150">
         <v>1</v>
       </c>
@@ -4110,11 +3725,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E151">
         <v>1</v>
       </c>
@@ -4135,11 +3745,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E152">
         <v>448</v>
       </c>
@@ -4160,11 +3765,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E153">
         <v>1</v>
       </c>
@@ -4185,11 +3785,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E154">
         <v>3</v>
       </c>
@@ -4210,11 +3805,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E155">
         <v>5</v>
       </c>
@@ -4235,11 +3825,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D156" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E156">
         <v>47</v>
       </c>
@@ -4260,11 +3845,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E157">
         <v>3</v>
       </c>
@@ -4310,11 +3890,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E159">
         <v>8</v>
       </c>
@@ -4335,11 +3910,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D160" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E160">
         <v>2</v>
       </c>
@@ -4360,11 +3930,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D161" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E161">
         <v>1</v>
       </c>
@@ -4385,11 +3950,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E162">
         <v>1</v>
       </c>
@@ -4435,11 +3995,6 @@
           <t>Austria</t>
         </is>
       </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E164">
         <v>2</v>
       </c>
@@ -4485,11 +4040,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D166" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E166">
         <v>65</v>
       </c>
@@ -4635,11 +4185,6 @@
           <t>Ireland</t>
         </is>
       </c>
-      <c r="D172" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E172">
         <v>1</v>
       </c>
@@ -4685,11 +4230,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D174" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E174">
         <v>1</v>
       </c>
@@ -4710,11 +4250,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E175">
         <v>49</v>
       </c>
@@ -4735,11 +4270,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E176">
         <v>14</v>
       </c>
@@ -4760,11 +4290,6 @@
           <t>Architecture</t>
         </is>
       </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E177">
         <v>1</v>
       </c>
@@ -4785,11 +4310,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D178" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E178">
         <v>1</v>
       </c>
@@ -4910,11 +4430,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D183" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E183">
         <v>3</v>
       </c>
@@ -4935,11 +4450,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D184" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E184">
         <v>1</v>
       </c>
@@ -4960,11 +4470,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D185" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E185">
         <v>3</v>
       </c>
@@ -4985,11 +4490,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D186" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E186">
         <v>185</v>
       </c>
@@ -5010,11 +4510,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D187" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E187">
         <v>22</v>
       </c>
@@ -5035,11 +4530,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D188" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E188">
         <v>1</v>
       </c>
@@ -5060,11 +4550,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D189" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E189">
         <v>3</v>
       </c>
@@ -5085,11 +4570,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D190" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E190">
         <v>18</v>
       </c>
@@ -5110,11 +4590,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D191" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E191">
         <v>26</v>
       </c>
@@ -5135,11 +4610,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D192" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E192">
         <v>1</v>
       </c>
@@ -5160,11 +4630,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D193" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E193">
         <v>124</v>
       </c>
@@ -5185,11 +4650,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D194" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E194">
         <v>14</v>
       </c>
@@ -5210,11 +4670,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D195" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E195">
         <v>30</v>
       </c>
@@ -5235,11 +4690,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D196" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E196">
         <v>1</v>
       </c>
@@ -5260,11 +4710,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D197" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E197">
         <v>4</v>
       </c>
@@ -5285,11 +4730,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D198" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E198">
         <v>5</v>
       </c>
@@ -5310,11 +4750,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D199" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E199">
         <v>7</v>
       </c>
@@ -5335,11 +4770,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D200" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E200">
         <v>3</v>
       </c>
@@ -5360,11 +4790,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D201" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E201">
         <v>1</v>
       </c>
@@ -5410,11 +4835,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D203" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E203">
         <v>76</v>
       </c>
@@ -5435,11 +4855,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D204" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E204">
         <v>1</v>
       </c>
@@ -5460,11 +4875,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D205" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E205">
         <v>7</v>
       </c>
@@ -5485,11 +4895,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D206" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E206">
         <v>2</v>
       </c>
@@ -5510,11 +4915,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D207" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E207">
         <v>8</v>
       </c>
@@ -5535,11 +4935,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D208" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E208">
         <v>3</v>
       </c>
@@ -5560,11 +4955,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D209" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E209">
         <v>1</v>
       </c>
@@ -5585,11 +4975,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D210" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E210">
         <v>6</v>
       </c>
@@ -5610,11 +4995,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D211" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E211">
         <v>94</v>
       </c>
@@ -5635,11 +5015,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D212" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E212">
         <v>6</v>
       </c>
@@ -5660,11 +5035,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D213" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E213">
         <v>170</v>
       </c>
@@ -5685,11 +5055,6 @@
           <t>Brazil</t>
         </is>
       </c>
-      <c r="D214" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E214">
         <v>3</v>
       </c>
@@ -5710,11 +5075,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D215" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E215">
         <v>24</v>
       </c>
@@ -5735,11 +5095,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D216" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E216">
         <v>1</v>
       </c>
@@ -5760,11 +5115,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D217" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E217">
         <v>1</v>
       </c>
@@ -5785,11 +5135,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D218" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E218">
         <v>1</v>
       </c>
@@ -5810,11 +5155,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D219" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E219">
         <v>3</v>
       </c>
@@ -5835,11 +5175,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D220" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E220">
         <v>10</v>
       </c>
@@ -5885,11 +5220,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D222" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E222">
         <v>12</v>
       </c>
@@ -5935,11 +5265,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D224" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E224">
         <v>1</v>
       </c>
@@ -5960,11 +5285,6 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="D225" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E225">
         <v>1</v>
       </c>
@@ -6010,11 +5330,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D227" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E227">
         <v>2</v>
       </c>
@@ -6035,11 +5350,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D228" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E228">
         <v>2</v>
       </c>
@@ -6060,11 +5370,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D229" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E229">
         <v>103</v>
       </c>
@@ -6085,11 +5390,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D230" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E230">
         <v>2</v>
       </c>
@@ -6160,11 +5460,6 @@
           <t>Mexico</t>
         </is>
       </c>
-      <c r="D233" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E233">
         <v>1</v>
       </c>
@@ -6235,11 +5530,6 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="D236" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E236">
         <v>1</v>
       </c>
@@ -6260,11 +5550,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D237" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E237">
         <v>2</v>
       </c>
@@ -6285,11 +5570,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D238" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E238">
         <v>1</v>
       </c>
@@ -6360,11 +5640,6 @@
           <t>Brazil</t>
         </is>
       </c>
-      <c r="D241" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E241">
         <v>1</v>
       </c>
@@ -6460,11 +5735,6 @@
           <t>Brazil</t>
         </is>
       </c>
-      <c r="D245" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E245">
         <v>1</v>
       </c>
@@ -6485,11 +5755,6 @@
           <t>Switzerland</t>
         </is>
       </c>
-      <c r="D246" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E246">
         <v>1</v>
       </c>
@@ -6510,11 +5775,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D247" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E247">
         <v>1</v>
       </c>
@@ -6585,11 +5845,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D250" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E250">
         <v>1</v>
       </c>
@@ -6610,11 +5865,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D251" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E251">
         <v>2</v>
       </c>
@@ -6660,11 +5910,6 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="D253" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E253">
         <v>3</v>
       </c>
@@ -6810,11 +6055,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D259" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E259">
         <v>9</v>
       </c>
@@ -6835,11 +6075,6 @@
           <t>Belgium</t>
         </is>
       </c>
-      <c r="D260" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E260">
         <v>1</v>
       </c>
@@ -7135,11 +6370,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D272" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E272">
         <v>1</v>
       </c>
@@ -7210,11 +6440,6 @@
           <t>Turkey</t>
         </is>
       </c>
-      <c r="D275" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E275">
         <v>1</v>
       </c>
@@ -7235,11 +6460,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D276" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E276">
         <v>80</v>
       </c>
@@ -7285,11 +6505,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D278" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E278">
         <v>4</v>
       </c>
@@ -7335,11 +6550,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D280" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E280">
         <v>1</v>
       </c>
@@ -7360,11 +6570,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D281" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E281">
         <v>1</v>
       </c>
@@ -7435,11 +6640,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D284" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E284">
         <v>1</v>
       </c>
@@ -7485,11 +6685,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D286" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E286">
         <v>164</v>
       </c>
@@ -7535,11 +6730,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D288" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E288">
         <v>5</v>
       </c>
@@ -7585,11 +6775,6 @@
           <t>Vatican</t>
         </is>
       </c>
-      <c r="D290" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E290">
         <v>2</v>
       </c>
@@ -7610,11 +6795,6 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="D291" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E291">
         <v>6</v>
       </c>
@@ -7735,11 +6915,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D296" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E296">
         <v>1</v>
       </c>
@@ -7835,11 +7010,6 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="D300" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E300">
         <v>1</v>
       </c>
@@ -7860,11 +7030,6 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="D301" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E301">
         <v>1</v>
       </c>
@@ -7910,11 +7075,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D303" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E303">
         <v>2</v>
       </c>
@@ -7935,11 +7095,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D304" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E304">
         <v>1</v>
       </c>
@@ -7960,11 +7115,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D305" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E305">
         <v>1</v>
       </c>
@@ -8035,11 +7185,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D308" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E308">
         <v>9</v>
       </c>
@@ -8060,11 +7205,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D309" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E309">
         <v>1</v>
       </c>
@@ -8085,11 +7225,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D310" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E310">
         <v>2</v>
       </c>
@@ -8185,11 +7320,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D314" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E314">
         <v>256</v>
       </c>
@@ -8210,11 +7340,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D315" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E315">
         <v>6</v>
       </c>
@@ -8235,11 +7360,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D316" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E316">
         <v>3</v>
       </c>
@@ -8260,11 +7380,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D317" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E317">
         <v>1</v>
       </c>
@@ -8285,11 +7400,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D318" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E318">
         <v>10</v>
       </c>
@@ -8310,11 +7420,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D319" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E319">
         <v>119</v>
       </c>
@@ -8335,11 +7440,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D320" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E320">
         <v>4</v>
       </c>
@@ -8360,11 +7460,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D321" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E321">
         <v>1</v>
       </c>
@@ -8410,11 +7505,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D323" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E323">
         <v>1</v>
       </c>
@@ -8435,11 +7525,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D324" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E324">
         <v>2</v>
       </c>
@@ -8460,11 +7545,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D325" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E325">
         <v>1</v>
       </c>
@@ -8485,11 +7565,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D326" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E326">
         <v>1</v>
       </c>
@@ -8510,11 +7585,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D327" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E327">
         <v>52</v>
       </c>
@@ -8560,11 +7630,6 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="D329" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E329">
         <v>1</v>
       </c>
@@ -8585,11 +7650,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D330" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E330">
         <v>1</v>
       </c>
@@ -8610,11 +7670,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D331" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E331">
         <v>7</v>
       </c>
@@ -8635,11 +7690,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D332" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E332">
         <v>7</v>
       </c>
@@ -8660,11 +7710,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D333" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E333">
         <v>1</v>
       </c>
@@ -8685,11 +7730,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D334" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E334">
         <v>1</v>
       </c>
@@ -8735,11 +7775,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D336" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E336">
         <v>9</v>
       </c>
@@ -8760,11 +7795,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D337" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E337">
         <v>26</v>
       </c>
@@ -8810,11 +7840,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D339" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E339">
         <v>1</v>
       </c>
@@ -8835,11 +7860,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D340" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E340">
         <v>3</v>
       </c>
@@ -8885,11 +7905,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D342" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E342">
         <v>1</v>
       </c>
@@ -8910,11 +7925,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D343" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E343">
         <v>3</v>
       </c>
@@ -8935,11 +7945,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D344" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E344">
         <v>1</v>
       </c>
@@ -8960,11 +7965,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D345" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E345">
         <v>1</v>
       </c>
@@ -8985,11 +7985,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D346" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E346">
         <v>1</v>
       </c>
@@ -9010,11 +8005,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D347" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E347">
         <v>2</v>
       </c>
@@ -9035,11 +8025,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D348" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E348">
         <v>1</v>
       </c>
@@ -9135,11 +8120,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D352" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E352">
         <v>4</v>
       </c>
@@ -9160,11 +8140,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D353" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E353">
         <v>289</v>
       </c>
@@ -9185,11 +8160,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D354" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E354">
         <v>6</v>
       </c>
@@ -9210,11 +8180,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D355" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E355">
         <v>1</v>
       </c>
@@ -9235,11 +8200,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D356" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E356">
         <v>3</v>
       </c>
@@ -9260,11 +8220,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D357" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E357">
         <v>8</v>
       </c>
@@ -9285,11 +8240,6 @@
           <t>Liechtenstein</t>
         </is>
       </c>
-      <c r="D358" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E358">
         <v>1</v>
       </c>
@@ -9360,11 +8310,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D361" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E361">
         <v>1</v>
       </c>
@@ -9385,11 +8330,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D362" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E362">
         <v>2</v>
       </c>
@@ -9410,11 +8350,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D363" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E363">
         <v>1</v>
       </c>
@@ -9460,11 +8395,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D365" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E365">
         <v>2</v>
       </c>
@@ -9535,11 +8465,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D368" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E368">
         <v>4</v>
       </c>
@@ -9660,11 +8585,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D373" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E373">
         <v>5</v>
       </c>
@@ -9685,11 +8605,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D374" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E374">
         <v>2</v>
       </c>
@@ -9785,11 +8700,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D378" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E378">
         <v>6</v>
       </c>
@@ -9885,11 +8795,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D382" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E382">
         <v>7</v>
       </c>
@@ -9960,11 +8865,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D385" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E385">
         <v>1</v>
       </c>
@@ -9985,11 +8885,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D386" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E386">
         <v>10</v>
       </c>
@@ -10010,11 +8905,6 @@
           <t>Netherlands</t>
         </is>
       </c>
-      <c r="D387" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E387">
         <v>1</v>
       </c>
@@ -10035,11 +8925,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D388" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E388">
         <v>1</v>
       </c>
@@ -10060,11 +8945,6 @@
           <t>New Zealand</t>
         </is>
       </c>
-      <c r="D389" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E389">
         <v>1</v>
       </c>
@@ -10185,11 +9065,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D394" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E394">
         <v>1</v>
       </c>
@@ -10235,11 +9110,6 @@
           <t>India</t>
         </is>
       </c>
-      <c r="D396" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E396">
         <v>1</v>
       </c>
@@ -10260,11 +9130,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D397" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E397">
         <v>2</v>
       </c>
@@ -10310,11 +9175,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D399" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E399">
         <v>2</v>
       </c>
@@ -10335,11 +9195,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D400" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E400">
         <v>2</v>
       </c>
@@ -10360,11 +9215,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D401" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E401">
         <v>5</v>
       </c>
@@ -10410,11 +9260,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D403" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E403">
         <v>1</v>
       </c>
@@ -10460,11 +9305,6 @@
           <t>Croatia</t>
         </is>
       </c>
-      <c r="D405" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E405">
         <v>1</v>
       </c>
@@ -10485,11 +9325,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D406" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E406">
         <v>4</v>
       </c>
@@ -10510,11 +9345,6 @@
           <t>Brazil</t>
         </is>
       </c>
-      <c r="D407" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E407">
         <v>1</v>
       </c>
@@ -10560,11 +9390,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D409" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E409">
         <v>1</v>
       </c>
@@ -10585,11 +9410,6 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="D410" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E410">
         <v>2</v>
       </c>
@@ -10610,11 +9430,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D411" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E411">
         <v>12</v>
       </c>
@@ -10660,11 +9475,6 @@
           <t>Sweden</t>
         </is>
       </c>
-      <c r="D413" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E413">
         <v>1</v>
       </c>
@@ -10685,11 +9495,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D414" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E414">
         <v>13</v>
       </c>
@@ -10760,11 +9565,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D417" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E417">
         <v>1</v>
       </c>
@@ -10810,11 +9610,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D419" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E419">
         <v>9</v>
       </c>
@@ -10835,11 +9630,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D420" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E420">
         <v>1</v>
       </c>
@@ -10860,11 +9650,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D421" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E421">
         <v>1</v>
       </c>
@@ -10885,11 +9670,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D422" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E422">
         <v>3</v>
       </c>
@@ -10905,11 +9685,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D423" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E423">
         <v>2</v>
       </c>
@@ -11050,11 +9825,6 @@
           <t>Poland</t>
         </is>
       </c>
-      <c r="D429" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E429">
         <v>2</v>
       </c>
@@ -11075,11 +9845,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D430" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E430">
         <v>27</v>
       </c>
@@ -11220,11 +9985,6 @@
           <t>Serbia</t>
         </is>
       </c>
-      <c r="D436" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E436">
         <v>1</v>
       </c>
@@ -11295,11 +10055,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D439" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E439">
         <v>10</v>
       </c>
@@ -11320,11 +10075,6 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="D440" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E440">
         <v>3</v>
       </c>
@@ -11370,11 +10120,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D442" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E442">
         <v>1</v>
       </c>
@@ -11395,11 +10140,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D443" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E443">
         <v>1</v>
       </c>
@@ -11420,11 +10160,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D444" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E444">
         <v>3</v>
       </c>
@@ -11440,11 +10175,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D445" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E445">
         <v>59</v>
       </c>
@@ -11460,11 +10190,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D446" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E446">
         <v>1</v>
       </c>
@@ -11560,11 +10285,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D450" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E450">
         <v>1</v>
       </c>
@@ -11660,11 +10380,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D454" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E454">
         <v>9</v>
       </c>
@@ -11685,11 +10400,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D455" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E455">
         <v>1</v>
       </c>
@@ -11705,11 +10415,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D456" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E456">
         <v>4</v>
       </c>
@@ -11730,11 +10435,6 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="D457" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E457">
         <v>1</v>
       </c>
@@ -12030,11 +10730,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D469" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E469">
         <v>2</v>
       </c>
@@ -12050,11 +10745,6 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="D470" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E470">
         <v>1</v>
       </c>
@@ -12125,11 +10815,6 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="D473" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E473">
         <v>1</v>
       </c>
@@ -12175,11 +10860,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D475" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E475">
         <v>1</v>
       </c>
@@ -12195,11 +10875,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D476" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E476">
         <v>2</v>
       </c>
@@ -12220,11 +10895,6 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="D477" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E477">
         <v>1</v>
       </c>
@@ -12245,11 +10915,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D478" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E478">
         <v>1</v>
       </c>
@@ -12265,11 +10930,6 @@
           <t>Poland</t>
         </is>
       </c>
-      <c r="D479" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E479">
         <v>8</v>
       </c>
@@ -12465,11 +11125,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D487" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E487">
         <v>2</v>
       </c>
@@ -12510,11 +11165,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D489" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E489">
         <v>2</v>
       </c>
@@ -12555,11 +11205,6 @@
           <t>Slovenia</t>
         </is>
       </c>
-      <c r="D491" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E491">
         <v>1</v>
       </c>
@@ -12625,11 +11270,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D494" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E494">
         <v>1</v>
       </c>
@@ -12775,11 +11415,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D500" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E500">
         <v>1</v>
       </c>
@@ -12800,11 +11435,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D501" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E501">
         <v>10</v>
       </c>
@@ -12950,11 +11580,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D507" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E507">
         <v>1</v>
       </c>
@@ -13045,11 +11670,6 @@
           <t>New Zealand</t>
         </is>
       </c>
-      <c r="D511" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E511">
         <v>1</v>
       </c>
@@ -13070,11 +11690,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D512" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E512">
         <v>2</v>
       </c>
@@ -13095,11 +11710,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D513" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E513">
         <v>1</v>
       </c>
@@ -13115,11 +11725,6 @@
           <t>Sweden</t>
         </is>
       </c>
-      <c r="D514" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E514">
         <v>1</v>
       </c>
@@ -13140,11 +11745,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D515" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E515">
         <v>1</v>
       </c>
@@ -13165,11 +11765,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D516" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E516">
         <v>1</v>
       </c>
@@ -13190,11 +11785,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D517" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E517">
         <v>3</v>
       </c>
@@ -13235,11 +11825,6 @@
           <t>Poland</t>
         </is>
       </c>
-      <c r="D519" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E519">
         <v>2</v>
       </c>
@@ -13360,11 +11945,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D524" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E524">
         <v>1</v>
       </c>
@@ -13480,11 +12060,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D529" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E529">
         <v>1</v>
       </c>
@@ -13500,11 +12075,6 @@
           <t>Belgium</t>
         </is>
       </c>
-      <c r="D530" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E530">
         <v>1</v>
       </c>
@@ -13570,11 +12140,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D533" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E533">
         <v>1</v>
       </c>
@@ -13590,11 +12155,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D534" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E534">
         <v>1</v>
       </c>
@@ -13615,11 +12175,6 @@
           <t>Canada</t>
         </is>
       </c>
-      <c r="D535" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E535">
         <v>1</v>
       </c>
@@ -13640,11 +12195,6 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="D536" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E536">
         <v>9</v>
       </c>
@@ -13665,11 +12215,6 @@
           <t>Ireland</t>
         </is>
       </c>
-      <c r="D537" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E537">
         <v>1</v>
       </c>
@@ -13765,11 +12310,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D541" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E541">
         <v>1</v>
       </c>
@@ -13790,11 +12330,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D542" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E542">
         <v>2</v>
       </c>
@@ -13815,11 +12350,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D543" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E543">
         <v>2</v>
       </c>
@@ -13840,11 +12370,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D544" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E544">
         <v>2</v>
       </c>
@@ -13865,11 +12390,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D545" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E545">
         <v>2</v>
       </c>
@@ -13915,11 +12435,6 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="D547" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E547">
         <v>4</v>
       </c>
@@ -13940,11 +12455,6 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="D548" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E548">
         <v>5</v>
       </c>
@@ -14040,11 +12550,6 @@
           <t>Malta</t>
         </is>
       </c>
-      <c r="D552" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E552">
         <v>1</v>
       </c>
@@ -14060,11 +12565,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D553" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E553">
         <v>1</v>
       </c>
@@ -14310,11 +12810,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D563" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E563">
         <v>1</v>
       </c>
@@ -14335,11 +12830,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D564" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E564">
         <v>2</v>
       </c>
@@ -14460,11 +12950,6 @@
           <t>Brazil</t>
         </is>
       </c>
-      <c r="D569" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E569">
         <v>1</v>
       </c>
@@ -14485,11 +12970,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D570" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E570">
         <v>1</v>
       </c>
@@ -14585,11 +13065,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D574" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E574">
         <v>2</v>
       </c>
@@ -14610,11 +13085,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D575" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E575">
         <v>1</v>
       </c>
@@ -14635,11 +13105,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D576" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E576">
         <v>1</v>
       </c>
@@ -14660,11 +13125,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D577" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E577">
         <v>1</v>
       </c>
@@ -14685,11 +13145,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D578" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E578">
         <v>1</v>
       </c>
@@ -14760,11 +13215,6 @@
           <t>Vatican</t>
         </is>
       </c>
-      <c r="D581" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E581">
         <v>1</v>
       </c>
@@ -14785,11 +13235,6 @@
           <t>Vatican</t>
         </is>
       </c>
-      <c r="D582" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E582">
         <v>4</v>
       </c>
@@ -15010,11 +13455,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D591" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E591">
         <v>1</v>
       </c>
@@ -15035,11 +13475,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D592" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E592">
         <v>2</v>
       </c>
@@ -15060,11 +13495,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D593" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E593">
         <v>1</v>
       </c>
@@ -15085,11 +13515,6 @@
           <t>India</t>
         </is>
       </c>
-      <c r="D594" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E594">
         <v>1</v>
       </c>
@@ -15160,11 +13585,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D597" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E597">
         <v>1</v>
       </c>
@@ -15210,11 +13630,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D599" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E599">
         <v>1</v>
       </c>
@@ -15260,11 +13675,6 @@
           <t>China</t>
         </is>
       </c>
-      <c r="D601" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E601">
         <v>1</v>
       </c>
@@ -15285,11 +13695,6 @@
           <t>Portugal</t>
         </is>
       </c>
-      <c r="D602" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E602">
         <v>1</v>
       </c>
@@ -15335,11 +13740,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D604" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E604">
         <v>1</v>
       </c>
@@ -15385,11 +13785,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D606" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E606">
         <v>1</v>
       </c>
@@ -15410,11 +13805,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D607" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E607">
         <v>12</v>
       </c>
@@ -15435,11 +13825,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D608" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E608">
         <v>135</v>
       </c>
@@ -15460,11 +13845,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D609" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E609">
         <v>1</v>
       </c>
@@ -15585,11 +13965,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D614" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E614">
         <v>1</v>
       </c>
@@ -15685,11 +14060,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D618" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E618">
         <v>1</v>
       </c>
@@ -15735,11 +14105,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D620" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E620">
         <v>1</v>
       </c>
@@ -15760,11 +14125,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="D621" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E621">
         <v>1</v>
       </c>
@@ -15810,11 +14170,6 @@
           <t>France</t>
         </is>
       </c>
-      <c r="D623" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E623">
         <v>4</v>
       </c>
@@ -15835,11 +14190,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D624" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E624">
         <v>1</v>
       </c>
@@ -15860,11 +14210,6 @@
           <t>Italy</t>
         </is>
       </c>
-      <c r="D625" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E625">
         <v>1</v>
       </c>
@@ -15910,11 +14255,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D627" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E627">
         <v>1</v>
       </c>
@@ -16010,11 +14350,6 @@
           <t>Poland</t>
         </is>
       </c>
-      <c r="D631" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E631">
         <v>2</v>
       </c>
@@ -16035,11 +14370,6 @@
           <t>Germany</t>
         </is>
       </c>
-      <c r="D632" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E632">
         <v>1</v>
       </c>
@@ -16060,11 +14390,6 @@
           <t>Spain</t>
         </is>
       </c>
-      <c r="D633" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="E633">
         <v>1</v>
       </c>
@@ -16083,11 +14408,6 @@
       <c r="C634" t="inlineStr">
         <is>
           <t>Spain</t>
-        </is>
-      </c>
-      <c r="D634" t="inlineStr">
-        <is>
-          <t>NA</t>
         </is>
       </c>
       <c r="E634">

</xml_diff>